<commit_message>
Cleaned up frontend files
</commit_message>
<xml_diff>
--- a/Other files/Tables For Prod.xlsx
+++ b/Other files/Tables For Prod.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\TheQBCarousel\Other files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DE658EF-6E89-4552-A497-602A6B934496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{613F4D62-EC3E-4403-ABE4-6B2407201B7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="833" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="833" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IDsInfo" sheetId="9" r:id="rId1"/>
-    <sheet name="Teams" sheetId="1" r:id="rId2"/>
+    <sheet name="teams" sheetId="1" r:id="rId2"/>
     <sheet name="Players" sheetId="3" r:id="rId3"/>
     <sheet name="conferences" sheetId="14" r:id="rId4"/>
     <sheet name="Roles" sheetId="15" r:id="rId5"/>
@@ -35,7 +35,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Players!$A$1:$C$87</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Teams!$A$1:$I$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">teams!$A$1:$I$33</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="327">
   <si>
     <t>TeamID</t>
   </si>
@@ -902,9 +902,6 @@
     <t>Malik Cunningham</t>
   </si>
   <si>
-    <t>INSERT INTO the_qb_carousel.Players(PlayerID,Name,IsActive) VALUES</t>
-  </si>
-  <si>
     <t>PJ Walker</t>
   </si>
   <si>
@@ -1059,6 +1056,9 @@
   </si>
   <si>
     <t>Password Reset</t>
+  </si>
+  <si>
+    <t>INSERT INTO players(PlayerID,Name,IsActive) VALUES</t>
   </si>
 </sst>
 </file>
@@ -1779,7 +1779,7 @@
         <v>118</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -3454,16 +3454,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>286</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -3972,10 +3972,10 @@
         <v>74</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>288</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>289</v>
       </c>
     </row>
   </sheetData>
@@ -4003,22 +4003,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>295</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>112</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>297</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -4026,13 +4026,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -4047,13 +4047,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -4068,13 +4068,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>299</v>
+      </c>
+      <c r="C4" t="s">
         <v>300</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>301</v>
-      </c>
-      <c r="D4" t="s">
-        <v>302</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -4089,13 +4089,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>323</v>
+      </c>
+      <c r="C5" t="s">
         <v>324</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>325</v>
-      </c>
-      <c r="D5" t="s">
-        <v>326</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -4126,119 +4126,119 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>306</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E3" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C4" t="s">
         <v>240</v>
       </c>
       <c r="D4" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
+        <v>310</v>
+      </c>
+      <c r="C5" t="s">
         <v>311</v>
       </c>
-      <c r="C5" t="s">
-        <v>312</v>
-      </c>
       <c r="D5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E5" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
+        <v>313</v>
+      </c>
+      <c r="C6" t="s">
         <v>314</v>
       </c>
-      <c r="C6" t="s">
-        <v>315</v>
-      </c>
       <c r="D6" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E6" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C7" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E7" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
+        <v>320</v>
+      </c>
+      <c r="C8" t="s">
         <v>321</v>
       </c>
-      <c r="C8" t="s">
-        <v>322</v>
-      </c>
       <c r="D8" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E8" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C9" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D9" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E9" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
   </sheetData>
@@ -4261,10 +4261,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L65"/>
+  <dimension ref="A1:L64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4307,14 +4307,14 @@
         <v>220</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L1" t="str">
-        <f>"INSERT INTO the_qb_carousel.teams ("&amp;_xlfn.TEXTJOIN(",",FALSE,A1:J1)&amp;") VALUES"</f>
-        <v>INSERT INTO the_qb_carousel.teams (TeamID,Season,Location,Nickname,Conference,Division,IsActive,GridColumn,GridRow,DefaultPlayerID) VALUES</v>
+        <f>"INSERT INTO teams ("&amp;_xlfn.TEXTJOIN(",",FALSE,A1:J1)&amp;") VALUES"</f>
+        <v>INSERT INTO teams (TeamID,Season,Location,Nickname,Conference,Division,IsActive,GridColumn,GridRow,DefaultPlayerID) VALUES</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -4345,9 +4345,12 @@
       <c r="I2">
         <v>2</v>
       </c>
+      <c r="J2" s="6">
+        <v>53</v>
+      </c>
       <c r="L2" t="str">
-        <f>"("&amp;A2&amp;",'"&amp;_xlfn.TEXTJOIN("','",FALSE,B2:F2)&amp;"',"&amp;G2&amp;","&amp;H2&amp;","&amp;I2&amp;","&amp;IF(LEN(J2)&gt;0,J2,"NULL")&amp;")"&amp;IF(LEN(A3)&gt;0,",","")</f>
-        <v>(1,'2022','Baltimore','Ravens','AFC','North',1,2,2,NULL),</v>
+        <f>"("&amp;A2&amp;",'"&amp;_xlfn.TEXTJOIN("','",FALSE,B2:F2)&amp;"',"&amp;G2&amp;","&amp;H2&amp;","&amp;I2&amp;","&amp;IF(LEN(J2)&gt;0,J2,"NULL")&amp;")"&amp;IF(LEN(A3)&gt;0,",",";")</f>
+        <v>(1,'2022','Baltimore','Ravens','AFC','North',1,2,2,53),</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -4378,9 +4381,12 @@
       <c r="I3">
         <v>3</v>
       </c>
+      <c r="J3" s="6">
+        <v>39</v>
+      </c>
       <c r="L3" t="str">
-        <f t="shared" ref="L3:L65" si="0">"("&amp;A3&amp;",'"&amp;_xlfn.TEXTJOIN("','",FALSE,B3:F3)&amp;"',"&amp;G3&amp;","&amp;H3&amp;","&amp;I3&amp;","&amp;IF(LEN(J3)&gt;0,J3,"NULL")&amp;")"&amp;IF(LEN(A4)&gt;0,",","")</f>
-        <v>(2,'2022','Cincinnati','Bengals','AFC','North',1,2,3,NULL),</v>
+        <f t="shared" ref="L3:L33" si="0">"("&amp;A3&amp;",'"&amp;_xlfn.TEXTJOIN("','",FALSE,B3:F3)&amp;"',"&amp;G3&amp;","&amp;H3&amp;","&amp;I3&amp;","&amp;IF(LEN(J3)&gt;0,J3,"NULL")&amp;")"&amp;IF(LEN(A4)&gt;0,",",";")</f>
+        <v>(2,'2022','Cincinnati','Bengals','AFC','North',1,2,3,39),</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -4411,9 +4417,12 @@
       <c r="I4">
         <v>4</v>
       </c>
+      <c r="J4">
+        <v>22</v>
+      </c>
       <c r="L4" t="str">
         <f t="shared" si="0"/>
-        <v>(3,'2022','Cleveland','Browns','AFC','North',1,2,4,NULL),</v>
+        <v>(3,'2022','Cleveland','Browns','AFC','North',1,2,4,22),</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -4444,9 +4453,12 @@
       <c r="I5">
         <v>5</v>
       </c>
+      <c r="J5">
+        <v>90</v>
+      </c>
       <c r="L5" t="str">
         <f t="shared" si="0"/>
-        <v>(4,'2022','Pittsburgh','Steelers','AFC','North',1,2,5,NULL),</v>
+        <v>(4,'2022','Pittsburgh','Steelers','AFC','North',1,2,5,90),</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
@@ -4477,9 +4489,12 @@
       <c r="I6">
         <v>2</v>
       </c>
+      <c r="J6" s="6">
+        <v>43</v>
+      </c>
       <c r="L6" t="str">
         <f t="shared" si="0"/>
-        <v>(5,'2022','Buffalo','Bills','AFC','East',1,3,2,NULL),</v>
+        <v>(5,'2022','Buffalo','Bills','AFC','East',1,3,2,43),</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
@@ -4510,9 +4525,12 @@
       <c r="I7">
         <v>3</v>
       </c>
+      <c r="J7" s="6">
+        <v>83</v>
+      </c>
       <c r="L7" t="str">
         <f t="shared" si="0"/>
-        <v>(6,'2022','Miami','Dolphins','AFC','East',1,3,3,NULL),</v>
+        <v>(6,'2022','Miami','Dolphins','AFC','East',1,3,3,83),</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
@@ -4543,9 +4561,12 @@
       <c r="I8">
         <v>4</v>
       </c>
+      <c r="J8" s="6">
+        <v>55</v>
+      </c>
       <c r="L8" t="str">
         <f t="shared" si="0"/>
-        <v>(7,'2022','New England','Patriots','AFC','East',1,3,4,NULL),</v>
+        <v>(7,'2022','New England','Patriots','AFC','East',1,3,4,55),</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
@@ -4576,9 +4597,12 @@
       <c r="I9">
         <v>5</v>
       </c>
+      <c r="J9" s="6">
+        <v>86</v>
+      </c>
       <c r="L9" t="str">
         <f t="shared" si="0"/>
-        <v>(8,'2022','New York','Jets','AFC','East',1,3,5,NULL),</v>
+        <v>(8,'2022','New York','Jets','AFC','East',1,3,5,86),</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
@@ -4609,9 +4633,12 @@
       <c r="I10">
         <v>2</v>
       </c>
+      <c r="J10" s="6">
+        <v>20</v>
+      </c>
       <c r="L10" t="str">
         <f t="shared" si="0"/>
-        <v>(9,'2022','Houston','Texans','AFC','South',1,4,2,NULL),</v>
+        <v>(9,'2022','Houston','Texans','AFC','South',1,4,2,20),</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
@@ -4642,9 +4669,12 @@
       <c r="I11">
         <v>3</v>
       </c>
+      <c r="J11">
+        <v>58</v>
+      </c>
       <c r="L11" t="str">
         <f t="shared" si="0"/>
-        <v>(10,'2022','Indianapolis','Colts','AFC','South',1,4,3,NULL),</v>
+        <v>(10,'2022','Indianapolis','Colts','AFC','South',1,4,3,58),</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
@@ -4675,9 +4705,12 @@
       <c r="I12">
         <v>4</v>
       </c>
+      <c r="J12" s="6">
+        <v>80</v>
+      </c>
       <c r="L12" t="str">
         <f t="shared" si="0"/>
-        <v>(11,'2022','Jacksonville','Jaguars','AFC','South',1,4,4,NULL),</v>
+        <v>(11,'2022','Jacksonville','Jaguars','AFC','South',1,4,4,80),</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
@@ -4708,9 +4741,12 @@
       <c r="I13">
         <v>5</v>
       </c>
+      <c r="J13" s="6">
+        <v>69</v>
+      </c>
       <c r="L13" t="str">
         <f t="shared" si="0"/>
-        <v>(12,'2022','Tennessee','Titans','AFC','South',1,4,5,NULL),</v>
+        <v>(12,'2022','Tennessee','Titans','AFC','South',1,4,5,69),</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
@@ -4741,9 +4777,12 @@
       <c r="I14">
         <v>2</v>
       </c>
+      <c r="J14">
+        <v>68</v>
+      </c>
       <c r="L14" t="str">
         <f t="shared" si="0"/>
-        <v>(13,'2022','Denver','Broncos','AFC','West',1,5,2,NULL),</v>
+        <v>(13,'2022','Denver','Broncos','AFC','West',1,5,2,68),</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
@@ -4774,9 +4813,12 @@
       <c r="I15">
         <v>3</v>
       </c>
+      <c r="J15" s="6">
+        <v>66</v>
+      </c>
       <c r="L15" t="str">
         <f t="shared" si="0"/>
-        <v>(14,'2022','Kansas City','Chiefs','AFC','West',1,5,3,NULL),</v>
+        <v>(14,'2022','Kansas City','Chiefs','AFC','West',1,5,3,66),</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
@@ -4807,9 +4849,12 @@
       <c r="I16">
         <v>4</v>
       </c>
+      <c r="J16" s="6">
+        <v>21</v>
+      </c>
       <c r="L16" t="str">
         <f t="shared" si="0"/>
-        <v>(15,'2022','Las Vegas','Raiders','AFC','West',1,5,4,NULL),</v>
+        <v>(15,'2022','Las Vegas','Raiders','AFC','West',1,5,4,21),</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
@@ -4840,9 +4885,12 @@
       <c r="I17">
         <v>5</v>
       </c>
+      <c r="J17" s="6">
+        <v>47</v>
+      </c>
       <c r="L17" t="str">
         <f t="shared" si="0"/>
-        <v>(16,'2022','Los Angeles','Chargers','AFC','West',1,5,5,NULL),</v>
+        <v>(16,'2022','Los Angeles','Chargers','AFC','West',1,5,5,47),</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
@@ -4873,9 +4921,12 @@
       <c r="I18">
         <v>6</v>
       </c>
+      <c r="J18" s="6">
+        <v>46</v>
+      </c>
       <c r="L18" t="str">
         <f t="shared" si="0"/>
-        <v>(17,'2022','Chicago','Bears','NFC','North',1,2,6,NULL),</v>
+        <v>(17,'2022','Chicago','Bears','NFC','North',1,2,6,46),</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
@@ -4906,9 +4957,12 @@
       <c r="I19">
         <v>7</v>
       </c>
+      <c r="J19" s="6">
+        <v>36</v>
+      </c>
       <c r="L19" t="str">
         <f t="shared" si="0"/>
-        <v>(18,'2022','Detroit','Lions','NFC','North',1,2,7,NULL),</v>
+        <v>(18,'2022','Detroit','Lions','NFC','North',1,2,7,36),</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
@@ -4939,9 +4993,12 @@
       <c r="I20">
         <v>8</v>
       </c>
+      <c r="J20" s="6">
+        <v>1</v>
+      </c>
       <c r="L20" t="str">
         <f t="shared" si="0"/>
-        <v>(19,'2022','Green Bay','Packers','NFC','North',1,2,8,NULL),</v>
+        <v>(19,'2022','Green Bay','Packers','NFC','North',1,2,8,1),</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
@@ -4972,9 +5029,12 @@
       <c r="I21">
         <v>9</v>
       </c>
+      <c r="J21" s="6">
+        <v>49</v>
+      </c>
       <c r="L21" t="str">
         <f t="shared" si="0"/>
-        <v>(20,'2022','Minnesota','Vikings','NFC','North',1,2,9,NULL),</v>
+        <v>(20,'2022','Minnesota','Vikings','NFC','North',1,2,9,49),</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
@@ -5005,9 +5065,12 @@
       <c r="I22">
         <v>6</v>
       </c>
+      <c r="J22" s="6">
+        <v>17</v>
+      </c>
       <c r="L22" t="str">
         <f t="shared" si="0"/>
-        <v>(21,'2022','Dallas','Cowboys','NFC','East',1,3,6,NULL),</v>
+        <v>(21,'2022','Dallas','Cowboys','NFC','East',1,3,6,17),</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
@@ -5038,9 +5101,12 @@
       <c r="I23">
         <v>7</v>
       </c>
+      <c r="J23" s="6">
+        <v>18</v>
+      </c>
       <c r="L23" t="str">
         <f t="shared" si="0"/>
-        <v>(22,'2022','New York','Giants','NFC','East',1,3,7,NULL),</v>
+        <v>(22,'2022','New York','Giants','NFC','East',1,3,7,18),</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
@@ -5071,9 +5137,12 @@
       <c r="I24">
         <v>8</v>
       </c>
+      <c r="J24" s="6">
+        <v>34</v>
+      </c>
       <c r="L24" t="str">
         <f t="shared" si="0"/>
-        <v>(23,'2022','Philadelphia','Eagles','NFC','East',1,3,8,NULL),</v>
+        <v>(23,'2022','Philadelphia','Eagles','NFC','East',1,3,8,34),</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
@@ -5104,9 +5173,12 @@
       <c r="I25">
         <v>9</v>
       </c>
+      <c r="J25">
+        <v>11</v>
+      </c>
       <c r="L25" t="str">
         <f t="shared" si="0"/>
-        <v>(24,'2022','Washington','Commanders','NFC','East',1,3,9,NULL),</v>
+        <v>(24,'2022','Washington','Commanders','NFC','East',1,3,9,11),</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
@@ -5137,9 +5209,12 @@
       <c r="I26">
         <v>6</v>
       </c>
+      <c r="J26">
+        <v>56</v>
+      </c>
       <c r="L26" t="str">
         <f t="shared" si="0"/>
-        <v>(25,'2022','Atlanta','Falcons','NFC','South',1,4,6,NULL),</v>
+        <v>(25,'2022','Atlanta','Falcons','NFC','South',1,4,6,56),</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
@@ -5170,9 +5245,12 @@
       <c r="I27">
         <v>7</v>
       </c>
+      <c r="J27" s="6">
+        <v>70</v>
+      </c>
       <c r="L27" t="str">
         <f t="shared" si="0"/>
-        <v>(26,'2022','Carolina','Panthers','NFC','South',1,4,7,NULL),</v>
+        <v>(26,'2022','Carolina','Panthers','NFC','South',1,4,7,70),</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
@@ -5203,9 +5281,12 @@
       <c r="I28">
         <v>8</v>
       </c>
+      <c r="J28" s="6">
+        <v>35</v>
+      </c>
       <c r="L28" t="str">
         <f t="shared" si="0"/>
-        <v>(27,'2022','New Orleans','Saints','NFC','South',1,4,8,NULL),</v>
+        <v>(27,'2022','New Orleans','Saints','NFC','South',1,4,8,35),</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
@@ -5236,9 +5317,12 @@
       <c r="I29">
         <v>9</v>
       </c>
+      <c r="J29" s="6">
+        <v>78</v>
+      </c>
       <c r="L29" t="str">
         <f t="shared" si="0"/>
-        <v>(28,'2022','Tampa Bay','Buccaneers','NFC','South',1,4,9,NULL),</v>
+        <v>(28,'2022','Tampa Bay','Buccaneers','NFC','South',1,4,9,78),</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
@@ -5269,9 +5353,12 @@
       <c r="I30">
         <v>6</v>
       </c>
+      <c r="J30" s="6">
+        <v>52</v>
+      </c>
       <c r="L30" t="str">
         <f t="shared" si="0"/>
-        <v>(29,'2022','Arizona','Cardinals','NFC','West',1,5,6,NULL),</v>
+        <v>(29,'2022','Arizona','Cardinals','NFC','West',1,5,6,52),</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
@@ -5302,9 +5389,12 @@
       <c r="I31">
         <v>7</v>
       </c>
+      <c r="J31" s="6">
+        <v>59</v>
+      </c>
       <c r="L31" t="str">
         <f t="shared" si="0"/>
-        <v>(30,'2022','Los Angeles','Rams','NFC','West',1,5,7,NULL),</v>
+        <v>(30,'2022','Los Angeles','Rams','NFC','West',1,5,7,59),</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
@@ -5335,9 +5425,12 @@
       <c r="I32">
         <v>8</v>
       </c>
+      <c r="J32" s="6">
+        <v>82</v>
+      </c>
       <c r="L32" t="str">
         <f t="shared" si="0"/>
-        <v>(31,'2022','San Francisco','49ers','NFC','West',1,5,8,NULL),</v>
+        <v>(31,'2022','San Francisco','49ers','NFC','West',1,5,8,82),</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
@@ -5368,1162 +5461,88 @@
       <c r="I33">
         <v>9</v>
       </c>
+      <c r="J33">
+        <v>29</v>
+      </c>
       <c r="L33" t="str">
         <f t="shared" si="0"/>
-        <v>(32,'2022','Seattle','Seahawks','NFC','West',1,5,9,NULL),</v>
+        <v>(32,'2022','Seattle','Seahawks','NFC','West',1,5,9,29);</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A34">
-        <v>33</v>
-      </c>
-      <c r="B34">
-        <v>2023</v>
-      </c>
-      <c r="C34" t="s">
-        <v>58</v>
-      </c>
-      <c r="D34" t="s">
-        <v>59</v>
-      </c>
-      <c r="E34" t="s">
-        <v>27</v>
-      </c>
-      <c r="F34" t="s">
-        <v>48</v>
-      </c>
-      <c r="G34">
-        <v>1</v>
-      </c>
-      <c r="H34">
-        <v>2</v>
-      </c>
-      <c r="I34">
-        <v>2</v>
-      </c>
-      <c r="J34" s="6">
-        <v>53</v>
-      </c>
-      <c r="L34" t="str">
-        <f t="shared" si="0"/>
-        <v>(33,'2023','Baltimore','Ravens','AFC','North',1,2,2,53),</v>
-      </c>
+      <c r="J34" s="6"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A35">
-        <v>34</v>
-      </c>
-      <c r="B35">
-        <v>2023</v>
-      </c>
-      <c r="C35" t="s">
-        <v>49</v>
-      </c>
-      <c r="D35" t="s">
-        <v>50</v>
-      </c>
-      <c r="E35" t="s">
-        <v>27</v>
-      </c>
-      <c r="F35" t="s">
-        <v>48</v>
-      </c>
-      <c r="G35">
-        <v>1</v>
-      </c>
-      <c r="H35">
-        <v>2</v>
-      </c>
-      <c r="I35">
-        <v>3</v>
-      </c>
-      <c r="J35" s="6">
-        <v>39</v>
-      </c>
-      <c r="L35" t="str">
-        <f t="shared" si="0"/>
-        <v>(34,'2023','Cincinnati','Bengals','AFC','North',1,2,3,39),</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A36">
-        <v>35</v>
-      </c>
-      <c r="B36">
-        <v>2023</v>
-      </c>
-      <c r="C36" t="s">
-        <v>51</v>
-      </c>
-      <c r="D36" t="s">
-        <v>52</v>
-      </c>
-      <c r="E36" t="s">
-        <v>27</v>
-      </c>
-      <c r="F36" t="s">
-        <v>48</v>
-      </c>
-      <c r="G36">
-        <v>1</v>
-      </c>
-      <c r="H36">
-        <v>2</v>
-      </c>
-      <c r="I36">
-        <v>4</v>
-      </c>
-      <c r="J36">
-        <v>22</v>
-      </c>
-      <c r="L36" t="str">
-        <f t="shared" si="0"/>
-        <v>(35,'2023','Cleveland','Browns','AFC','North',1,2,4,22),</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A37">
-        <v>36</v>
-      </c>
-      <c r="B37">
-        <v>2023</v>
-      </c>
-      <c r="C37" t="s">
-        <v>53</v>
-      </c>
-      <c r="D37" t="s">
-        <v>54</v>
-      </c>
-      <c r="E37" t="s">
-        <v>27</v>
-      </c>
-      <c r="F37" t="s">
-        <v>48</v>
-      </c>
-      <c r="G37">
-        <v>1</v>
-      </c>
-      <c r="H37">
-        <v>2</v>
-      </c>
-      <c r="I37">
-        <v>5</v>
-      </c>
-      <c r="J37">
-        <v>90</v>
-      </c>
-      <c r="L37" t="str">
-        <f t="shared" si="0"/>
-        <v>(36,'2023','Pittsburgh','Steelers','AFC','North',1,2,5,90),</v>
-      </c>
+      <c r="J35" s="6"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A38">
-        <v>37</v>
-      </c>
-      <c r="B38">
-        <v>2023</v>
-      </c>
-      <c r="C38" t="s">
-        <v>22</v>
-      </c>
-      <c r="D38" t="s">
-        <v>23</v>
-      </c>
-      <c r="E38" t="s">
-        <v>27</v>
-      </c>
-      <c r="F38" t="s">
-        <v>28</v>
-      </c>
-      <c r="G38">
-        <v>1</v>
-      </c>
-      <c r="H38">
-        <v>3</v>
-      </c>
-      <c r="I38">
-        <v>2</v>
-      </c>
-      <c r="J38" s="6">
-        <v>43</v>
-      </c>
-      <c r="L38" t="str">
-        <f t="shared" si="0"/>
-        <v>(37,'2023','Buffalo','Bills','AFC','East',1,3,2,43),</v>
-      </c>
+      <c r="J38" s="6"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A39">
-        <v>38</v>
-      </c>
-      <c r="B39">
-        <v>2023</v>
-      </c>
-      <c r="C39" t="s">
-        <v>25</v>
-      </c>
-      <c r="D39" t="s">
-        <v>26</v>
-      </c>
-      <c r="E39" t="s">
-        <v>27</v>
-      </c>
-      <c r="F39" t="s">
-        <v>28</v>
-      </c>
-      <c r="G39">
-        <v>1</v>
-      </c>
-      <c r="H39">
-        <v>3</v>
-      </c>
-      <c r="I39">
-        <v>3</v>
-      </c>
-      <c r="J39" s="6">
-        <v>83</v>
-      </c>
-      <c r="L39" t="str">
-        <f t="shared" si="0"/>
-        <v>(38,'2023','Miami','Dolphins','AFC','East',1,3,3,83),</v>
-      </c>
+      <c r="J39" s="6"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A40">
-        <v>39</v>
-      </c>
-      <c r="B40">
-        <v>2023</v>
-      </c>
-      <c r="C40" t="s">
-        <v>24</v>
-      </c>
-      <c r="D40" t="s">
-        <v>120</v>
-      </c>
-      <c r="E40" t="s">
-        <v>27</v>
-      </c>
-      <c r="F40" t="s">
-        <v>28</v>
-      </c>
-      <c r="G40">
-        <v>1</v>
-      </c>
-      <c r="H40">
-        <v>3</v>
-      </c>
-      <c r="I40">
-        <v>4</v>
-      </c>
-      <c r="J40" s="6">
-        <v>55</v>
-      </c>
-      <c r="L40" t="str">
-        <f t="shared" si="0"/>
-        <v>(39,'2023','New England','Patriots','AFC','East',1,3,4,55),</v>
-      </c>
+      <c r="J40" s="6"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A41">
-        <v>40</v>
-      </c>
-      <c r="B41">
-        <v>2023</v>
-      </c>
-      <c r="C41" t="s">
-        <v>3</v>
-      </c>
-      <c r="D41" t="s">
-        <v>5</v>
-      </c>
-      <c r="E41" t="s">
-        <v>27</v>
-      </c>
-      <c r="F41" t="s">
-        <v>28</v>
-      </c>
-      <c r="G41">
-        <v>1</v>
-      </c>
-      <c r="H41">
-        <v>3</v>
-      </c>
-      <c r="I41">
-        <v>5</v>
-      </c>
-      <c r="J41" s="6">
-        <v>86</v>
-      </c>
-      <c r="L41" t="str">
-        <f t="shared" si="0"/>
-        <v>(40,'2023','New York','Jets','AFC','East',1,3,5,86),</v>
-      </c>
+      <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A42">
-        <v>41</v>
-      </c>
-      <c r="B42">
-        <v>2023</v>
-      </c>
-      <c r="C42" t="s">
-        <v>70</v>
-      </c>
-      <c r="D42" t="s">
-        <v>71</v>
-      </c>
-      <c r="E42" t="s">
-        <v>27</v>
-      </c>
-      <c r="F42" t="s">
-        <v>42</v>
-      </c>
-      <c r="G42">
-        <v>1</v>
-      </c>
-      <c r="H42">
-        <v>4</v>
-      </c>
-      <c r="I42">
-        <v>2</v>
-      </c>
-      <c r="J42" s="6">
-        <v>20</v>
-      </c>
-      <c r="L42" t="str">
-        <f t="shared" si="0"/>
-        <v>(41,'2023','Houston','Texans','AFC','South',1,4,2,20),</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A43">
-        <v>42</v>
-      </c>
-      <c r="B43">
-        <v>2023</v>
-      </c>
-      <c r="C43" t="s">
-        <v>119</v>
-      </c>
-      <c r="D43" t="s">
-        <v>55</v>
-      </c>
-      <c r="E43" t="s">
-        <v>27</v>
-      </c>
-      <c r="F43" t="s">
-        <v>42</v>
-      </c>
-      <c r="G43">
-        <v>1</v>
-      </c>
-      <c r="H43">
-        <v>4</v>
-      </c>
-      <c r="I43">
-        <v>3</v>
-      </c>
-      <c r="J43">
-        <v>58</v>
-      </c>
-      <c r="L43" t="str">
-        <f t="shared" si="0"/>
-        <v>(42,'2023','Indianapolis','Colts','AFC','South',1,4,3,58),</v>
-      </c>
+      <c r="J42" s="6"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A44">
-        <v>43</v>
-      </c>
-      <c r="B44">
-        <v>2023</v>
-      </c>
-      <c r="C44" t="s">
-        <v>60</v>
-      </c>
-      <c r="D44" t="s">
-        <v>61</v>
-      </c>
-      <c r="E44" t="s">
-        <v>27</v>
-      </c>
-      <c r="F44" t="s">
-        <v>42</v>
-      </c>
-      <c r="G44">
-        <v>1</v>
-      </c>
-      <c r="H44">
-        <v>4</v>
-      </c>
-      <c r="I44">
-        <v>4</v>
-      </c>
-      <c r="J44" s="6">
-        <v>80</v>
-      </c>
-      <c r="L44" t="str">
-        <f t="shared" si="0"/>
-        <v>(43,'2023','Jacksonville','Jaguars','AFC','South',1,4,4,80),</v>
-      </c>
+      <c r="J44" s="6"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A45">
-        <v>44</v>
-      </c>
-      <c r="B45">
-        <v>2023</v>
-      </c>
-      <c r="C45" t="s">
-        <v>56</v>
-      </c>
-      <c r="D45" t="s">
-        <v>57</v>
-      </c>
-      <c r="E45" t="s">
-        <v>27</v>
-      </c>
-      <c r="F45" t="s">
-        <v>42</v>
-      </c>
-      <c r="G45">
-        <v>1</v>
-      </c>
-      <c r="H45">
-        <v>4</v>
-      </c>
-      <c r="I45">
-        <v>5</v>
-      </c>
-      <c r="J45" s="6">
-        <v>69</v>
-      </c>
-      <c r="L45" t="str">
-        <f t="shared" si="0"/>
-        <v>(44,'2023','Tennessee','Titans','AFC','South',1,4,5,69),</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A46">
-        <v>45</v>
-      </c>
-      <c r="B46">
-        <v>2023</v>
-      </c>
-      <c r="C46" t="s">
-        <v>38</v>
-      </c>
-      <c r="D46" t="s">
-        <v>39</v>
-      </c>
-      <c r="E46" t="s">
-        <v>27</v>
-      </c>
-      <c r="F46" t="s">
-        <v>16</v>
-      </c>
-      <c r="G46">
-        <v>1</v>
-      </c>
-      <c r="H46">
-        <v>5</v>
-      </c>
-      <c r="I46">
-        <v>2</v>
-      </c>
-      <c r="J46">
-        <v>68</v>
-      </c>
-      <c r="L46" t="str">
-        <f t="shared" si="0"/>
-        <v>(45,'2023','Denver','Broncos','AFC','West',1,5,2,68),</v>
-      </c>
+      <c r="J45" s="6"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A47">
-        <v>46</v>
-      </c>
-      <c r="B47">
-        <v>2023</v>
-      </c>
-      <c r="C47" t="s">
-        <v>36</v>
-      </c>
-      <c r="D47" t="s">
-        <v>37</v>
-      </c>
-      <c r="E47" t="s">
-        <v>27</v>
-      </c>
-      <c r="F47" t="s">
-        <v>16</v>
-      </c>
-      <c r="G47">
-        <v>1</v>
-      </c>
-      <c r="H47">
-        <v>5</v>
-      </c>
-      <c r="I47">
-        <v>3</v>
-      </c>
-      <c r="J47" s="6">
-        <v>66</v>
-      </c>
-      <c r="L47" t="str">
-        <f t="shared" si="0"/>
-        <v>(46,'2023','Kansas City','Chiefs','AFC','West',1,5,3,66),</v>
-      </c>
+      <c r="J47" s="6"/>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A48">
-        <v>47</v>
-      </c>
-      <c r="B48">
-        <v>2023</v>
-      </c>
-      <c r="C48" t="s">
-        <v>40</v>
-      </c>
-      <c r="D48" t="s">
-        <v>41</v>
-      </c>
-      <c r="E48" t="s">
-        <v>27</v>
-      </c>
-      <c r="F48" t="s">
-        <v>16</v>
-      </c>
-      <c r="G48">
-        <v>1</v>
-      </c>
-      <c r="H48">
-        <v>5</v>
-      </c>
-      <c r="I48">
-        <v>4</v>
-      </c>
-      <c r="J48" s="6">
-        <v>21</v>
-      </c>
-      <c r="L48" t="str">
-        <f t="shared" si="0"/>
-        <v>(47,'2023','Las Vegas','Raiders','AFC','West',1,5,4,21),</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A49">
-        <v>48</v>
-      </c>
-      <c r="B49">
-        <v>2023</v>
-      </c>
-      <c r="C49" t="s">
-        <v>6</v>
-      </c>
-      <c r="D49" t="s">
-        <v>8</v>
-      </c>
-      <c r="E49" t="s">
-        <v>27</v>
-      </c>
-      <c r="F49" t="s">
-        <v>16</v>
-      </c>
-      <c r="G49">
-        <v>1</v>
-      </c>
-      <c r="H49">
-        <v>5</v>
-      </c>
-      <c r="I49">
-        <v>5</v>
-      </c>
-      <c r="J49" s="6">
-        <v>47</v>
-      </c>
-      <c r="L49" t="str">
-        <f t="shared" si="0"/>
-        <v>(48,'2023','Los Angeles','Chargers','AFC','West',1,5,5,47),</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A50">
-        <v>49</v>
-      </c>
-      <c r="B50">
-        <v>2023</v>
-      </c>
-      <c r="C50" t="s">
-        <v>43</v>
-      </c>
-      <c r="D50" t="s">
-        <v>44</v>
-      </c>
-      <c r="E50" t="s">
-        <v>15</v>
-      </c>
-      <c r="F50" t="s">
-        <v>48</v>
-      </c>
-      <c r="G50">
-        <v>1</v>
-      </c>
-      <c r="H50">
-        <v>2</v>
-      </c>
-      <c r="I50">
-        <v>6</v>
-      </c>
-      <c r="J50" s="6">
-        <v>46</v>
-      </c>
-      <c r="L50" t="str">
-        <f t="shared" si="0"/>
-        <v>(49,'2023','Chicago','Bears','NFC','North',1,2,6,46),</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A51">
-        <v>50</v>
-      </c>
-      <c r="B51">
-        <v>2023</v>
-      </c>
-      <c r="C51" t="s">
-        <v>45</v>
-      </c>
-      <c r="D51" t="s">
-        <v>46</v>
-      </c>
-      <c r="E51" t="s">
-        <v>15</v>
-      </c>
-      <c r="F51" t="s">
-        <v>48</v>
-      </c>
-      <c r="G51">
-        <v>1</v>
-      </c>
-      <c r="H51">
-        <v>2</v>
-      </c>
-      <c r="I51">
-        <v>7</v>
-      </c>
-      <c r="J51" s="6">
-        <v>36</v>
-      </c>
-      <c r="L51" t="str">
-        <f t="shared" si="0"/>
-        <v>(50,'2023','Detroit','Lions','NFC','North',1,2,7,36),</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A52">
-        <v>51</v>
-      </c>
-      <c r="B52">
-        <v>2023</v>
-      </c>
-      <c r="C52" t="s">
-        <v>11</v>
-      </c>
-      <c r="D52" t="s">
-        <v>29</v>
-      </c>
-      <c r="E52" t="s">
-        <v>15</v>
-      </c>
-      <c r="F52" t="s">
-        <v>48</v>
-      </c>
-      <c r="G52">
-        <v>1</v>
-      </c>
-      <c r="H52">
-        <v>2</v>
-      </c>
-      <c r="I52">
-        <v>8</v>
-      </c>
-      <c r="J52" s="6">
-        <v>1</v>
-      </c>
-      <c r="L52" t="str">
-        <f t="shared" si="0"/>
-        <v>(51,'2023','Green Bay','Packers','NFC','North',1,2,8,1),</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A53">
-        <v>52</v>
-      </c>
-      <c r="B53">
-        <v>2023</v>
-      </c>
-      <c r="C53" t="s">
-        <v>9</v>
-      </c>
-      <c r="D53" t="s">
-        <v>10</v>
-      </c>
-      <c r="E53" t="s">
-        <v>15</v>
-      </c>
-      <c r="F53" t="s">
-        <v>48</v>
-      </c>
-      <c r="G53">
-        <v>1</v>
-      </c>
-      <c r="H53">
-        <v>2</v>
-      </c>
-      <c r="I53">
-        <v>9</v>
-      </c>
-      <c r="J53" s="6">
-        <v>49</v>
-      </c>
-      <c r="L53" t="str">
-        <f t="shared" si="0"/>
-        <v>(52,'2023','Minnesota','Vikings','NFC','North',1,2,9,49),</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A54">
-        <v>53</v>
-      </c>
-      <c r="B54">
-        <v>2023</v>
-      </c>
-      <c r="C54" t="s">
-        <v>20</v>
-      </c>
-      <c r="D54" t="s">
-        <v>21</v>
-      </c>
-      <c r="E54" t="s">
-        <v>15</v>
-      </c>
-      <c r="F54" t="s">
-        <v>28</v>
-      </c>
-      <c r="G54">
-        <v>1</v>
-      </c>
-      <c r="H54">
-        <v>3</v>
-      </c>
-      <c r="I54">
-        <v>6</v>
-      </c>
-      <c r="J54" s="6">
-        <v>17</v>
-      </c>
-      <c r="L54" t="str">
-        <f t="shared" si="0"/>
-        <v>(53,'2023','Dallas','Cowboys','NFC','East',1,3,6,17),</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A55">
-        <v>54</v>
-      </c>
-      <c r="B55">
-        <v>2023</v>
-      </c>
-      <c r="C55" t="s">
-        <v>3</v>
-      </c>
-      <c r="D55" t="s">
-        <v>4</v>
-      </c>
-      <c r="E55" t="s">
-        <v>15</v>
-      </c>
-      <c r="F55" t="s">
-        <v>28</v>
-      </c>
-      <c r="G55">
-        <v>1</v>
-      </c>
-      <c r="H55">
-        <v>3</v>
-      </c>
-      <c r="I55">
-        <v>7</v>
-      </c>
-      <c r="J55" s="6">
-        <v>18</v>
-      </c>
-      <c r="L55" t="str">
-        <f t="shared" si="0"/>
-        <v>(54,'2023','New York','Giants','NFC','East',1,3,7,18),</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A56">
-        <v>55</v>
-      </c>
-      <c r="B56">
-        <v>2023</v>
-      </c>
-      <c r="C56" t="s">
-        <v>18</v>
-      </c>
-      <c r="D56" t="s">
-        <v>19</v>
-      </c>
-      <c r="E56" t="s">
-        <v>15</v>
-      </c>
-      <c r="F56" t="s">
-        <v>28</v>
-      </c>
-      <c r="G56">
-        <v>1</v>
-      </c>
-      <c r="H56">
-        <v>3</v>
-      </c>
-      <c r="I56">
-        <v>8</v>
-      </c>
-      <c r="J56" s="6">
-        <v>34</v>
-      </c>
-      <c r="L56" t="str">
-        <f t="shared" si="0"/>
-        <v>(55,'2023','Philadelphia','Eagles','NFC','East',1,3,8,34),</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A57">
-        <v>56</v>
-      </c>
-      <c r="B57">
-        <v>2023</v>
-      </c>
-      <c r="C57" t="s">
-        <v>17</v>
-      </c>
-      <c r="D57" t="s">
-        <v>121</v>
-      </c>
-      <c r="E57" t="s">
-        <v>15</v>
-      </c>
-      <c r="F57" t="s">
-        <v>28</v>
-      </c>
-      <c r="G57">
-        <v>1</v>
-      </c>
-      <c r="H57">
-        <v>3</v>
-      </c>
-      <c r="I57">
-        <v>9</v>
-      </c>
-      <c r="J57">
-        <v>11</v>
-      </c>
-      <c r="L57" t="str">
-        <f t="shared" si="0"/>
-        <v>(56,'2023','Washington','Commanders','NFC','East',1,3,9,11),</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A58">
-        <v>57</v>
-      </c>
-      <c r="B58">
-        <v>2023</v>
-      </c>
-      <c r="C58" t="s">
-        <v>64</v>
-      </c>
-      <c r="D58" t="s">
-        <v>65</v>
-      </c>
-      <c r="E58" t="s">
-        <v>15</v>
-      </c>
-      <c r="F58" t="s">
-        <v>42</v>
-      </c>
-      <c r="G58">
-        <v>1</v>
-      </c>
-      <c r="H58">
-        <v>4</v>
-      </c>
-      <c r="I58">
-        <v>6</v>
-      </c>
-      <c r="J58">
-        <v>56</v>
-      </c>
-      <c r="L58" t="str">
-        <f t="shared" si="0"/>
-        <v>(57,'2023','Atlanta','Falcons','NFC','South',1,4,6,56),</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A59">
-        <v>58</v>
-      </c>
-      <c r="B59">
-        <v>2023</v>
-      </c>
-      <c r="C59" t="s">
-        <v>68</v>
-      </c>
-      <c r="D59" t="s">
-        <v>69</v>
-      </c>
-      <c r="E59" t="s">
-        <v>15</v>
-      </c>
-      <c r="F59" t="s">
-        <v>42</v>
-      </c>
-      <c r="G59">
-        <v>1</v>
-      </c>
-      <c r="H59">
-        <v>4</v>
-      </c>
-      <c r="I59">
-        <v>7</v>
-      </c>
-      <c r="J59" s="6">
-        <v>70</v>
-      </c>
-      <c r="L59" t="str">
-        <f t="shared" si="0"/>
-        <v>(58,'2023','Carolina','Panthers','NFC','South',1,4,7,70),</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A60">
-        <v>59</v>
-      </c>
-      <c r="B60">
-        <v>2023</v>
-      </c>
-      <c r="C60" t="s">
-        <v>66</v>
-      </c>
-      <c r="D60" t="s">
-        <v>67</v>
-      </c>
-      <c r="E60" t="s">
-        <v>15</v>
-      </c>
-      <c r="F60" t="s">
-        <v>42</v>
-      </c>
-      <c r="G60">
-        <v>1</v>
-      </c>
-      <c r="H60">
-        <v>4</v>
-      </c>
-      <c r="I60">
-        <v>8</v>
-      </c>
-      <c r="J60" s="6">
-        <v>35</v>
-      </c>
-      <c r="L60" t="str">
-        <f t="shared" si="0"/>
-        <v>(59,'2023','New Orleans','Saints','NFC','South',1,4,8,35),</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A61">
-        <v>60</v>
-      </c>
-      <c r="B61">
-        <v>2023</v>
-      </c>
-      <c r="C61" t="s">
-        <v>62</v>
-      </c>
-      <c r="D61" t="s">
-        <v>63</v>
-      </c>
-      <c r="E61" t="s">
-        <v>15</v>
-      </c>
-      <c r="F61" t="s">
-        <v>42</v>
-      </c>
-      <c r="G61">
-        <v>1</v>
-      </c>
-      <c r="H61">
-        <v>4</v>
-      </c>
-      <c r="I61">
-        <v>9</v>
-      </c>
-      <c r="J61" s="6">
-        <v>78</v>
-      </c>
-      <c r="L61" t="str">
-        <f t="shared" si="0"/>
-        <v>(60,'2023','Tampa Bay','Buccaneers','NFC','South',1,4,9,78),</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A62">
-        <v>61</v>
-      </c>
-      <c r="B62">
-        <v>2023</v>
-      </c>
-      <c r="C62" t="s">
-        <v>30</v>
-      </c>
-      <c r="D62" t="s">
-        <v>31</v>
-      </c>
-      <c r="E62" t="s">
-        <v>15</v>
-      </c>
-      <c r="F62" t="s">
-        <v>16</v>
-      </c>
-      <c r="G62">
-        <v>1</v>
-      </c>
-      <c r="H62">
-        <v>5</v>
-      </c>
-      <c r="I62">
-        <v>6</v>
-      </c>
-      <c r="J62" s="6">
-        <v>52</v>
-      </c>
-      <c r="L62" t="str">
-        <f t="shared" si="0"/>
-        <v>(61,'2023','Arizona','Cardinals','NFC','West',1,5,6,52),</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A63">
-        <v>62</v>
-      </c>
-      <c r="B63">
-        <v>2023</v>
-      </c>
-      <c r="C63" t="s">
-        <v>6</v>
-      </c>
-      <c r="D63" t="s">
-        <v>7</v>
-      </c>
-      <c r="E63" t="s">
-        <v>15</v>
-      </c>
-      <c r="F63" t="s">
-        <v>16</v>
-      </c>
-      <c r="G63">
-        <v>1</v>
-      </c>
-      <c r="H63">
-        <v>5</v>
-      </c>
-      <c r="I63">
-        <v>7</v>
-      </c>
-      <c r="J63" s="6">
-        <v>59</v>
-      </c>
-      <c r="L63" t="str">
-        <f t="shared" si="0"/>
-        <v>(62,'2023','Los Angeles','Rams','NFC','West',1,5,7,59),</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A64">
-        <v>63</v>
-      </c>
-      <c r="B64">
-        <v>2023</v>
-      </c>
-      <c r="C64" t="s">
-        <v>32</v>
-      </c>
-      <c r="D64" t="s">
-        <v>33</v>
-      </c>
-      <c r="E64" t="s">
-        <v>15</v>
-      </c>
-      <c r="F64" t="s">
-        <v>16</v>
-      </c>
-      <c r="G64">
-        <v>1</v>
-      </c>
-      <c r="H64">
-        <v>5</v>
-      </c>
-      <c r="I64">
-        <v>8</v>
-      </c>
-      <c r="J64" s="6">
-        <v>82</v>
-      </c>
-      <c r="L64" t="str">
-        <f t="shared" si="0"/>
-        <v>(63,'2023','San Francisco','49ers','NFC','West',1,5,8,82),</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A65">
-        <v>64</v>
-      </c>
-      <c r="B65">
-        <v>2023</v>
-      </c>
-      <c r="C65" t="s">
-        <v>34</v>
-      </c>
-      <c r="D65" t="s">
-        <v>35</v>
-      </c>
-      <c r="E65" t="s">
-        <v>15</v>
-      </c>
-      <c r="F65" t="s">
-        <v>16</v>
-      </c>
-      <c r="G65">
-        <v>1</v>
-      </c>
-      <c r="H65">
-        <v>5</v>
-      </c>
-      <c r="I65">
-        <v>9</v>
-      </c>
-      <c r="J65">
-        <v>29</v>
-      </c>
-      <c r="L65" t="str">
-        <f t="shared" si="0"/>
-        <v>(64,'2023','Seattle','Seahawks','NFC','West',1,5,9,29)</v>
-      </c>
+      <c r="J48" s="6"/>
+    </row>
+    <row r="49" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J49" s="6"/>
+    </row>
+    <row r="50" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J50" s="6"/>
+    </row>
+    <row r="51" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J51" s="6"/>
+    </row>
+    <row r="52" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J52" s="6"/>
+    </row>
+    <row r="53" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J53" s="6"/>
+    </row>
+    <row r="54" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J54" s="6"/>
+    </row>
+    <row r="55" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J55" s="6"/>
+    </row>
+    <row r="56" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J56" s="6"/>
+    </row>
+    <row r="59" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J59" s="6"/>
+    </row>
+    <row r="60" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J60" s="6"/>
+    </row>
+    <row r="61" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J61" s="6"/>
+    </row>
+    <row r="62" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J62" s="6"/>
+    </row>
+    <row r="63" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J63" s="6"/>
+    </row>
+    <row r="64" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J64" s="6"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:I33" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
@@ -6542,8 +5561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB509DC1-998D-4BFD-AC70-46B5E715D944}">
   <dimension ref="A1:L105"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="B96" sqref="B96"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="C105" sqref="C105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6563,7 +5582,7 @@
         <v>85</v>
       </c>
       <c r="E1" t="s">
-        <v>274</v>
+        <v>326</v>
       </c>
       <c r="I1" s="7"/>
       <c r="J1" s="7"/>
@@ -7789,7 +6808,7 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C66">
         <v>1</v>
@@ -8522,7 +7541,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F39725DE-07BC-4AA5-8629-15CC6A71CDD6}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
@@ -8891,7 +7910,7 @@
         <v>85</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J1" t="str" cm="1">
         <f t="array" aca="1" ref="J1" ca="1">"INSERT INTO the_qb_carousel."&amp;MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)&amp;"("&amp;_xlfn.TEXTJOIN(",",FALSE,A1:H1)&amp;") VALUES"</f>
@@ -9363,7 +8382,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C12" s="3">
         <v>45177.013888888891</v>
@@ -9381,7 +8400,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C13" s="3">
         <v>45298.895833333336</v>
@@ -9399,7 +8418,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C14" s="3">
         <v>45333.979166666664</v>
@@ -9417,7 +8436,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C15" s="3">
         <v>45365.833333333336</v>
@@ -9435,7 +8454,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C16" s="3">
         <v>45408</v>

</xml_diff>